<commit_message>
Removed research time excel.
</commit_message>
<xml_diff>
--- a/Alessio_taxonomy_quantifier.xlsx
+++ b/Alessio_taxonomy_quantifier.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Dropbox/Classes/CS1950/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alessio/Documents/School/Research/Research_repo/research/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Quantifier" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="74">
   <si>
     <t>Appearance : Content : Entire Page : page is blank</t>
   </si>
@@ -204,13 +204,58 @@
   </si>
   <si>
     <t>Thoughts on Detection</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>Impossible</t>
+  </si>
+  <si>
+    <t>Check dom?</t>
+  </si>
+  <si>
+    <t>Look for key words</t>
+  </si>
+  <si>
+    <t>Check if JS exists?</t>
+  </si>
+  <si>
+    <t>Check for popup</t>
+  </si>
+  <si>
+    <t>Check if set to visible</t>
+  </si>
+  <si>
+    <t>Check which player being used</t>
+  </si>
+  <si>
+    <t>Check for icons?</t>
+  </si>
+  <si>
+    <t>Easy/Hard</t>
+  </si>
+  <si>
+    <t>Can fonts be checked?</t>
+  </si>
+  <si>
+    <t>Can original resolution be checked against current resolution?</t>
+  </si>
+  <si>
+    <t>Check before and after login?</t>
+  </si>
+  <si>
+    <t>Check before and after</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -222,12 +267,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
@@ -235,9 +274,19 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="20"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -262,19 +311,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,308 +646,580 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="84.83203125" customWidth="1"/>
+    <col min="1" max="1" width="98.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="B10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="B13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="B18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="B19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="B20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="B21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="B23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="B24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="B25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="B26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="B27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="B28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="B29" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="B30" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="B31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="B32" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="B33" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="B34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="B35" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="B36" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="B37" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="B38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="B39" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="B40" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="B41" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="B42" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="B43" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="B44" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="B45" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="B46" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="4"/>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="B47" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+      <c r="B48" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="B49" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+      <c r="B50" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="B51" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="4"/>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+      <c r="B52" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="4"/>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+      <c r="B53" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+      <c r="B54" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="4"/>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="B55" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+      <c r="B56" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="4"/>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
     </row>
   </sheetData>

</xml_diff>